<commit_message>
change grip and ori add sum
</commit_message>
<xml_diff>
--- a/help/grip_and_ori_a.xlsx
+++ b/help/grip_and_ori_a.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24870" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11550"/>
   </bookViews>
   <sheets>
     <sheet name="svod" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Сведения о сроках проведения лабораторных исследований от момента забора пробы (биоматериала) у пациента до выдачи результата исследования (в абсолютных числах количество проб)</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>А1.3</t>
+  </si>
+  <si>
+    <t>ИТОГО</t>
   </si>
 </sst>
 </file>
@@ -135,12 +138,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -230,7 +239,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -241,6 +250,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -587,10 +599,10 @@
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,37 +616,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
@@ -662,7 +674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
         <v>7</v>
@@ -675,6 +687,27 @@
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6">
+        <f>SUM(B8:B713)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" ref="C7:E7" si="0">SUM(C8:C713)</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>